<commit_message>
Kenntnisse und CV angepasst
</commit_message>
<xml_diff>
--- a/CV.xlsx
+++ b/CV.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/silviooberholzer/Documents/Bewerbungen/Meine/aktuell/CV_Visual/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/silviooberholzer/Documents/Bewerbungen/Meine/aktuell/CV_Visual/cv-streamlit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F096FEB6-0576-1F44-A9ED-C42691483FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F743E5C-58A8-6E4E-AEC0-57CFF16C2F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" xr2:uid="{A562BE8D-8BD6-4B69-B3A4-0A22EF180B3C}"/>
   </bookViews>
@@ -178,15 +178,6 @@
 • Berufsmaturität (Abschlussnote: 5.3)</t>
   </si>
   <si>
-    <t>berufsbegleitendes Betriebswirtschaftsstudium
-• Vertiefungsrichtung Rechnungswesen und Controlling (Abschlussnote: 5.5)
-• Bachelorthesis: Unternehmensbewertung und Nachfolgeregelung für Ostschweizer KMU (Note: 5.8)</t>
-  </si>
-  <si>
-    <t>berufsbegleitendes Studium Information and Data Science
-• Masterthesis: Datengetriebenes Belastungsmanagement für den FC St.Gallen (Note: 5.5; Abschlussnote: 5.3)</t>
-  </si>
-  <si>
     <t xml:space="preserve">• Mitgliederverwaltung
 • Organisation von Anlässen
 • Versand der Rechnungen
@@ -250,6 +241,15 @@
   </si>
   <si>
     <t>Projektmanagement Weiterbildung (Hermes 5.1 Advanced)</t>
+  </si>
+  <si>
+    <t>berufsbegleitendes Betriebswirtschaftsstudium (Abschlussnote: 5.5)
+• Vertiefungsrichtung Rechnungswesen und Controlling
+• Bachelorthesis: Unternehmensbewertung und Nachfolgeregelung für Ostschweizer KMU (Note: 5.8)</t>
+  </si>
+  <si>
+    <t>berufsbegleitendes Studium Information and Data Science (Abschlussnote: 5.3)
+• Masterthesis: Datengetriebenes Belastungsmanagement für den FC St.Gallen (Note: 5.5)</t>
   </si>
 </sst>
 </file>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6950E39-7D10-4061-A048-B3D838651420}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -646,7 +646,7 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -672,7 +672,7 @@
         <v>41121</v>
       </c>
       <c r="H2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -686,7 +686,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="E3">
         <v>5.5</v>
@@ -698,7 +698,7 @@
         <v>43343</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -712,7 +712,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="F4" s="1">
         <v>44440</v>
@@ -721,7 +721,7 @@
         <v>45138</v>
       </c>
       <c r="H4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -745,7 +745,7 @@
         <v>41121</v>
       </c>
       <c r="H5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -769,7 +769,7 @@
         <v>43100</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -793,7 +793,7 @@
         <v>43404</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="64" x14ac:dyDescent="0.2">
@@ -817,7 +817,7 @@
         <v>44135</v>
       </c>
       <c r="H8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -831,7 +831,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1">
@@ -841,7 +841,7 @@
         <v>44316</v>
       </c>
       <c r="H9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="64" x14ac:dyDescent="0.2">
@@ -865,7 +865,7 @@
         <v>44834</v>
       </c>
       <c r="H10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="64" x14ac:dyDescent="0.2">
@@ -879,7 +879,7 @@
         <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1">
@@ -887,10 +887,10 @@
       </c>
       <c r="G11" s="1">
         <f ca="1">TODAY()</f>
-        <v>45799</v>
+        <v>45800</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -914,7 +914,7 @@
         <v>44561</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="64" x14ac:dyDescent="0.2">
@@ -928,7 +928,7 @@
         <v>17</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F13" s="1">
         <v>43952</v>
@@ -937,7 +937,7 @@
         <v>45747</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -948,7 +948,7 @@
         <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
         <v>34</v>
@@ -960,7 +960,7 @@
         <v>43804</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -968,13 +968,13 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F15" s="1">
         <v>44958</v>
@@ -983,7 +983,7 @@
         <v>45010</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>